<commit_message>
add SetValueDecimal and getValueAsDecimal
</commit_message>
<xml_diff>
--- a/Excelam.Tests/Files/Cells/InitSetManyCellType.xlsx
+++ b/Excelam.Tests/Files/Cells/InitSetManyCellType.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/70-yvlawy/Excelam/Dev/ExcelamSol/Excelam.Tests/Files/Cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F14B30F-2652-4947-B4D6-BD5E7C88FBE0}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6037790-7746-4D4E-925D-DC58CA104FFE}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="16365" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="15900" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>hello</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>style number exists</t>
+  </si>
+  <si>
+    <t>cell empty, set decimal: 12,34</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +582,11 @@
         <v>56.78</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>